<commit_message>
calculating and plotting harvest breakdown from SE alaska
</commit_message>
<xml_diff>
--- a/data/CSIS_SurveyData_Demographics.xlsx
+++ b/data/CSIS_SurveyData_Demographics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariegutgesell/Desktop/Wild Foods Repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35DC834-73D6-C34A-815C-8E6EF2DD439A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058EE0F1-A99E-E745-A1A8-D915E6ABBBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27520" windowHeight="16480" xr2:uid="{103305FF-19B9-A04C-9A73-AD9D59ED97E3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27520" windowHeight="16480" activeTab="1" xr2:uid="{103305FF-19B9-A04C-9A73-AD9D59ED97E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey_Summary" sheetId="1" r:id="rId1"/>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641CC169-AD3B-2649-9EC8-0D9E9C2E703B}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1828,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7C6250-0454-1242-8FEF-5BAB633824E4}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3060,7 +3060,7 @@
         <v>6</v>
       </c>
       <c r="B43">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="C43">
         <v>24</v>

</xml_diff>

<commit_message>
added lat/long for communities
</commit_message>
<xml_diff>
--- a/data/CSIS_SurveyData_Demographics.xlsx
+++ b/data/CSIS_SurveyData_Demographics.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariegutgesell/Desktop/Wild Foods Repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058EE0F1-A99E-E745-A1A8-D915E6ABBBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F6D864-2D8F-A543-A9D0-67D0E6EDBF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27520" windowHeight="16480" activeTab="1" xr2:uid="{103305FF-19B9-A04C-9A73-AD9D59ED97E3}"/>
+    <workbookView xWindow="31800" yWindow="1280" windowWidth="35400" windowHeight="20320" activeTab="1" xr2:uid="{103305FF-19B9-A04C-9A73-AD9D59ED97E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey_Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Comp_Survey_Demographics" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Comp_Survey_Demographics!$A$1:$I$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Comp_Survey_Demographics!$A$1:$K$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Survey_Summary!$A$1:$D$44</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="174">
   <si>
     <t>Community</t>
   </si>
@@ -286,9 +286,6 @@
     <t>A list of 569 dwelling units within the city limits, including float houses and harbor live-aboards was obtained from the City of Craig planner, and 120 dwelling units were identified in the Port Saint Nicholas Road area. Of this 608 were determined to be occupied by year-round residents. Surveys were completed with a random sample of 173 households. Twenty-three households could not be contacted and 14 declined to participate.</t>
   </si>
   <si>
-    <t xml:space="preserve">Research was conducted in Hyder during February 1988. A 100% (census) sample was attempted. Six households were unavailable during the interview period. With the September 1997 release of the database, revised conversion factors have been applied to these data to allow comparisons with survey data collected for 1996/97. NOTE: study dates say 01/01/1997-12/31/1997, so I think was done in 1987? not totally clear.. </t>
-  </si>
-  <si>
     <t>Research was conducted in Edna Bay during January 1988. A 100% (census) sample was attempted. One household was unavailable during the interview period. With the September 1997 release of the database, revised conversion factors have been applied to these data to allow comparisons with survey data collected for 1996/97</t>
   </si>
   <si>
@@ -557,6 +554,15 @@
   </si>
   <si>
     <t>One hundred thirty-nine of the 234 occupied households in the community were surveyed by the Yakutat Tlingit Tribe. Seven households were unable to be contacted and 13 households declined to be surveyed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research was conducted in Hyder during February 1988. A 100% (census) sample was attempted. Six households were unavailable during the interview period. With the September 1997 release of the database, revised conversion factors have been applied to these data to allow comparisons with survey data collected for 1996/97. </t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -919,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641CC169-AD3B-2649-9EC8-0D9E9C2E703B}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,7 +977,7 @@
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -1054,7 +1060,7 @@
         <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1165,13 +1171,13 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" t="s">
         <v>88</v>
       </c>
-      <c r="E12" t="s">
-        <v>89</v>
-      </c>
       <c r="F12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1225,13 +1231,13 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
         <v>96</v>
       </c>
-      <c r="E15" t="s">
-        <v>97</v>
-      </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1245,13 +1251,13 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
         <v>102</v>
       </c>
-      <c r="E16" t="s">
-        <v>103</v>
-      </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1285,13 +1291,13 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1305,13 +1311,13 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
         <v>107</v>
       </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1345,13 +1351,13 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1365,13 +1371,13 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" t="s">
         <v>115</v>
       </c>
-      <c r="E22" t="s">
-        <v>116</v>
-      </c>
       <c r="F22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1385,13 +1391,13 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
         <v>120</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>121</v>
-      </c>
-      <c r="F23" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1545,13 +1551,13 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E31">
         <v>1987</v>
       </c>
       <c r="F31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1565,13 +1571,13 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1585,10 +1591,10 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
@@ -1625,10 +1631,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
@@ -1645,13 +1651,13 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1665,13 +1671,13 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" t="s">
         <v>147</v>
       </c>
-      <c r="E37" t="s">
-        <v>148</v>
-      </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1705,10 +1711,10 @@
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
@@ -1745,10 +1751,10 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
@@ -1785,13 +1791,13 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1805,13 +1811,13 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" t="s">
         <v>167</v>
       </c>
-      <c r="E44" t="s">
-        <v>168</v>
-      </c>
       <c r="F44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1826,2136 +1832,2578 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7C6250-0454-1242-8FEF-5BAB633824E4}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="11" max="11" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>1987</v>
+        <v>57.481974999999998</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>-135.55937800000001</v>
       </c>
       <c r="D2">
-        <v>39</v>
+        <v>1984</v>
       </c>
       <c r="E2">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="F2">
-        <v>77.900000000000006</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" t="s">
-        <v>67</v>
+        <v>145</v>
+      </c>
+      <c r="G2">
+        <v>163</v>
+      </c>
+      <c r="H2">
+        <v>622</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>1987</v>
+        <v>57.481974999999998</v>
       </c>
       <c r="C3">
-        <v>64</v>
+        <v>-135.55937800000001</v>
       </c>
       <c r="D3">
-        <v>418</v>
+        <v>1987</v>
       </c>
       <c r="E3">
-        <v>255</v>
+        <v>46</v>
       </c>
       <c r="F3">
-        <v>1554.2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
+        <v>139</v>
+      </c>
+      <c r="G3">
+        <v>193</v>
+      </c>
+      <c r="H3">
+        <v>520.79999999999995</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4">
-        <v>1984</v>
+        <v>57.481974999999998</v>
       </c>
       <c r="C4">
-        <v>38</v>
+        <v>-135.55937800000001</v>
       </c>
       <c r="D4">
-        <v>145</v>
+        <v>1996</v>
       </c>
       <c r="E4">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="F4">
-        <v>622</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" t="s">
-        <v>67</v>
+        <v>161</v>
+      </c>
+      <c r="G4">
+        <v>267</v>
+      </c>
+      <c r="H4">
+        <v>580.9</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5">
-        <v>1987</v>
+        <v>57.481974999999998</v>
       </c>
       <c r="C5">
+        <v>-135.55937800000001</v>
+      </c>
+      <c r="D5">
+        <v>2012</v>
+      </c>
+      <c r="E5">
+        <v>51</v>
+      </c>
+      <c r="F5">
+        <v>122</v>
+      </c>
+      <c r="G5">
+        <v>143</v>
+      </c>
+      <c r="H5">
+        <v>342.1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>56.590992999999997</v>
+      </c>
+      <c r="C6">
+        <v>-133.01373799999999</v>
+      </c>
+      <c r="D6">
+        <v>1987</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>44.2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>56.008578999999997</v>
+      </c>
+      <c r="C7">
+        <v>-132.82534200000001</v>
+      </c>
+      <c r="D7">
+        <v>1987</v>
+      </c>
+      <c r="E7">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <v>120</v>
+      </c>
+      <c r="H7">
+        <v>185.9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>56.008578999999997</v>
+      </c>
+      <c r="C8">
+        <v>-132.82534200000001</v>
+      </c>
+      <c r="D8">
+        <v>1998</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>142</v>
+      </c>
+      <c r="H8">
+        <v>213</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="D5">
-        <v>139</v>
-      </c>
-      <c r="E5">
-        <v>193</v>
-      </c>
-      <c r="F5">
-        <v>520.79999999999995</v>
-      </c>
-      <c r="G5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
+      <c r="B9">
+        <v>55.478845999999997</v>
+      </c>
+      <c r="C9">
+        <v>-133.129256</v>
+      </c>
+      <c r="D9">
+        <v>1987</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>365</v>
+      </c>
+      <c r="G9">
+        <v>213</v>
+      </c>
+      <c r="H9">
+        <v>1182.3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>55.478845999999997</v>
+      </c>
+      <c r="C10">
+        <v>-133.129256</v>
+      </c>
+      <c r="D10">
+        <v>1997</v>
+      </c>
+      <c r="E10">
+        <v>173</v>
+      </c>
+      <c r="F10">
+        <v>608</v>
+      </c>
+      <c r="G10">
+        <v>502</v>
+      </c>
+      <c r="H10">
+        <v>1764.3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>55.953246</v>
+      </c>
+      <c r="C11">
+        <v>-133.65418</v>
+      </c>
+      <c r="D11">
+        <v>1987</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>66</v>
+      </c>
+      <c r="H11">
+        <v>69.3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>55.953246</v>
+      </c>
+      <c r="C12">
+        <v>-133.65418</v>
+      </c>
+      <c r="D12">
+        <v>1998</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>37</v>
+      </c>
+      <c r="H12">
+        <v>52.4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>58.191077</v>
+      </c>
+      <c r="C13">
+        <v>-136.346574</v>
+      </c>
+      <c r="D13">
+        <v>1987</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>41</v>
+      </c>
+      <c r="H13">
+        <v>59.9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <v>58.069583999999999</v>
+      </c>
+      <c r="C14">
+        <v>-135.50465199999999</v>
+      </c>
+      <c r="D14">
         <v>1996</v>
       </c>
-      <c r="C6">
-        <v>74</v>
-      </c>
-      <c r="D6">
-        <v>161</v>
-      </c>
-      <c r="E6">
-        <v>267</v>
-      </c>
-      <c r="F6">
-        <v>580.9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>2012</v>
-      </c>
-      <c r="C7">
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="D7">
-        <v>122</v>
-      </c>
-      <c r="E7">
-        <v>143</v>
-      </c>
-      <c r="F7">
-        <v>342.1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8">
-        <v>1987</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>44.2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9">
-        <v>1987</v>
-      </c>
-      <c r="C9">
-        <v>41</v>
-      </c>
-      <c r="D9">
-        <v>66</v>
-      </c>
-      <c r="E9">
-        <v>120</v>
-      </c>
-      <c r="F9">
-        <v>185.9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>1998</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <v>75</v>
-      </c>
-      <c r="E10">
-        <v>142</v>
-      </c>
-      <c r="F10">
-        <v>213</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11">
-        <v>1987</v>
-      </c>
-      <c r="C11">
-        <v>64</v>
-      </c>
-      <c r="D11">
-        <v>365</v>
-      </c>
-      <c r="E11">
-        <v>213</v>
-      </c>
-      <c r="F11">
-        <v>1182.3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12">
-        <v>1997</v>
-      </c>
-      <c r="C12">
-        <v>173</v>
-      </c>
-      <c r="D12">
+      <c r="H14">
+        <v>63.8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>58.420245999999999</v>
+      </c>
+      <c r="C15">
+        <v>-135.75467699999999</v>
+      </c>
+      <c r="D15">
+        <v>1987</v>
+      </c>
+      <c r="E15">
+        <v>35</v>
+      </c>
+      <c r="F15">
+        <v>65</v>
+      </c>
+      <c r="G15">
+        <v>91</v>
+      </c>
+      <c r="H15">
+        <v>152.30000000000001</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>59.233953</v>
+      </c>
+      <c r="C16">
+        <v>-135.455916</v>
+      </c>
+      <c r="D16">
+        <v>1983</v>
+      </c>
+      <c r="E16">
+        <v>147</v>
+      </c>
+      <c r="F16">
+        <v>660</v>
+      </c>
+      <c r="G16">
+        <v>425</v>
+      </c>
+      <c r="H16">
+        <v>1908.2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>59.233953</v>
+      </c>
+      <c r="C17">
+        <v>-135.455916</v>
+      </c>
+      <c r="D17">
+        <v>1987</v>
+      </c>
+      <c r="E17">
+        <v>62</v>
+      </c>
+      <c r="F17">
         <v>608</v>
       </c>
-      <c r="E12">
-        <v>502</v>
-      </c>
-      <c r="F12">
-        <v>1764.3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13">
-        <v>1987</v>
-      </c>
-      <c r="C13">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>21</v>
-      </c>
-      <c r="E13">
-        <v>66</v>
-      </c>
-      <c r="F13">
-        <v>69.3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14">
-        <v>1998</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>17</v>
-      </c>
-      <c r="E14">
-        <v>37</v>
-      </c>
-      <c r="F14">
-        <v>52.4</v>
-      </c>
-      <c r="G14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15">
-        <v>1987</v>
-      </c>
-      <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>41</v>
-      </c>
-      <c r="F15">
-        <v>59.9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16">
-        <v>1996</v>
-      </c>
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <v>15</v>
-      </c>
-      <c r="E16">
-        <v>51</v>
-      </c>
-      <c r="F16">
-        <v>63.8</v>
-      </c>
-      <c r="G16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>1987</v>
-      </c>
-      <c r="C17">
-        <v>35</v>
-      </c>
-      <c r="D17">
-        <v>65</v>
-      </c>
-      <c r="E17">
-        <v>91</v>
-      </c>
-      <c r="F17">
-        <v>152.30000000000001</v>
-      </c>
-      <c r="G17" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" t="s">
-        <v>67</v>
+      <c r="G17">
+        <v>181</v>
+      </c>
+      <c r="H17">
+        <v>1622.6</v>
       </c>
       <c r="I17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18">
-        <v>1983</v>
+        <v>59.233953</v>
       </c>
       <c r="C18">
-        <v>147</v>
+        <v>-135.455916</v>
       </c>
       <c r="D18">
-        <v>660</v>
+        <v>1996</v>
       </c>
       <c r="E18">
-        <v>425</v>
+        <v>92</v>
       </c>
       <c r="F18">
-        <v>1908.2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" t="s">
-        <v>67</v>
+        <v>787</v>
+      </c>
+      <c r="G18">
+        <v>254</v>
+      </c>
+      <c r="H18">
+        <v>2172.8000000000002</v>
       </c>
       <c r="I18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19">
-        <v>1987</v>
+        <v>59.233953</v>
       </c>
       <c r="C19">
+        <v>-135.455916</v>
+      </c>
+      <c r="D19">
+        <v>2012</v>
+      </c>
+      <c r="E19">
+        <v>132</v>
+      </c>
+      <c r="F19">
+        <v>818</v>
+      </c>
+      <c r="G19">
+        <v>310</v>
+      </c>
+      <c r="H19">
+        <v>1921.1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>55.490454999999997</v>
+      </c>
+      <c r="C20">
+        <v>-132.644925</v>
+      </c>
+      <c r="D20">
+        <v>1987</v>
+      </c>
+      <c r="E20">
+        <v>29</v>
+      </c>
+      <c r="F20">
+        <v>32</v>
+      </c>
+      <c r="G20">
+        <v>72</v>
+      </c>
+      <c r="H20">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>55.490454999999997</v>
+      </c>
+      <c r="C21">
+        <v>-132.644925</v>
+      </c>
+      <c r="D21">
+        <v>1998</v>
+      </c>
+      <c r="E21">
+        <v>46</v>
+      </c>
+      <c r="F21">
+        <v>59</v>
+      </c>
+      <c r="G21">
+        <v>121</v>
+      </c>
+      <c r="H21">
+        <v>155.19999999999999</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>58.112166999999999</v>
+      </c>
+      <c r="C22">
+        <v>-135.44164900000001</v>
+      </c>
+      <c r="D22">
+        <v>1985</v>
+      </c>
+      <c r="E22">
+        <v>71</v>
+      </c>
+      <c r="F22">
+        <v>280</v>
+      </c>
+      <c r="G22">
+        <v>227</v>
+      </c>
+      <c r="H22">
+        <v>895.2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>58.112166999999999</v>
+      </c>
+      <c r="C23">
+        <v>-135.44164900000001</v>
+      </c>
+      <c r="D23">
+        <v>1987</v>
+      </c>
+      <c r="E23">
         <v>62</v>
       </c>
-      <c r="D19">
-        <v>608</v>
-      </c>
-      <c r="E19">
-        <v>181</v>
-      </c>
-      <c r="F19">
-        <v>1622.6</v>
-      </c>
-      <c r="G19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <v>1996</v>
-      </c>
-      <c r="C20">
-        <v>92</v>
-      </c>
-      <c r="D20">
-        <v>787</v>
-      </c>
-      <c r="E20">
-        <v>254</v>
-      </c>
-      <c r="F20">
-        <v>2172.8000000000002</v>
-      </c>
-      <c r="G20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21">
-        <v>2012</v>
-      </c>
-      <c r="C21">
-        <v>132</v>
-      </c>
-      <c r="D21">
-        <v>818</v>
-      </c>
-      <c r="E21">
-        <v>310</v>
-      </c>
-      <c r="F21">
-        <v>1921.1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22">
-        <v>1987</v>
-      </c>
-      <c r="C22">
-        <v>29</v>
-      </c>
-      <c r="D22">
-        <v>32</v>
-      </c>
-      <c r="E22">
-        <v>72</v>
-      </c>
-      <c r="F22">
-        <v>79.400000000000006</v>
-      </c>
-      <c r="G22" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23">
-        <v>1998</v>
-      </c>
-      <c r="C23">
-        <v>46</v>
-      </c>
-      <c r="D23">
-        <v>59</v>
-      </c>
-      <c r="E23">
-        <v>121</v>
-      </c>
       <c r="F23">
-        <v>155.19999999999999</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" t="s">
-        <v>67</v>
+        <v>219</v>
+      </c>
+      <c r="G23">
+        <v>222</v>
+      </c>
+      <c r="H23">
+        <v>699.8</v>
       </c>
       <c r="I23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J23" t="s">
+        <v>67</v>
+      </c>
+      <c r="K23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
       <c r="B24">
-        <v>1985</v>
+        <v>58.112166999999999</v>
       </c>
       <c r="C24">
-        <v>71</v>
+        <v>-135.44164900000001</v>
       </c>
       <c r="D24">
+        <v>1996</v>
+      </c>
+      <c r="E24">
+        <v>77</v>
+      </c>
+      <c r="F24">
         <v>280</v>
       </c>
-      <c r="E24">
-        <v>227</v>
-      </c>
-      <c r="F24">
-        <v>895.2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" t="s">
-        <v>67</v>
+      <c r="G24">
+        <v>245</v>
+      </c>
+      <c r="H24">
+        <v>890.9</v>
       </c>
       <c r="I24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J24" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
       <c r="B25">
-        <v>1987</v>
+        <v>58.112166999999999</v>
       </c>
       <c r="C25">
-        <v>62</v>
+        <v>-135.44164900000001</v>
       </c>
       <c r="D25">
-        <v>219</v>
+        <v>2012</v>
       </c>
       <c r="E25">
-        <v>222</v>
+        <v>122</v>
       </c>
       <c r="F25">
-        <v>699.8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" t="s">
-        <v>67</v>
+        <v>280</v>
+      </c>
+      <c r="G25">
+        <v>319</v>
+      </c>
+      <c r="H25">
+        <v>732.1</v>
       </c>
       <c r="I25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26">
-        <v>1996</v>
+        <v>58.112166999999999</v>
       </c>
       <c r="C26">
-        <v>77</v>
+        <v>-135.44164900000001</v>
       </c>
       <c r="D26">
-        <v>280</v>
+        <v>2016</v>
       </c>
       <c r="E26">
-        <v>245</v>
+        <v>65</v>
       </c>
       <c r="F26">
-        <v>890.9</v>
-      </c>
-      <c r="G26" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" t="s">
-        <v>66</v>
+        <v>260</v>
+      </c>
+      <c r="G26">
+        <v>184</v>
+      </c>
+      <c r="H26">
+        <v>736</v>
       </c>
       <c r="I26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B27">
-        <v>2012</v>
+        <v>55.206918999999999</v>
       </c>
       <c r="C27">
-        <v>122</v>
+        <v>-132.82456199999999</v>
       </c>
       <c r="D27">
-        <v>280</v>
+        <v>1987</v>
       </c>
       <c r="E27">
-        <v>319</v>
+        <v>35</v>
       </c>
       <c r="F27">
-        <v>732.1</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" t="s">
-        <v>67</v>
+        <v>110</v>
+      </c>
+      <c r="G27">
+        <v>129</v>
+      </c>
+      <c r="H27">
+        <v>379.1</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B28">
-        <v>2016</v>
+        <v>55.206918999999999</v>
       </c>
       <c r="C28">
-        <v>65</v>
+        <v>-132.82456199999999</v>
       </c>
       <c r="D28">
-        <v>260</v>
+        <v>1997</v>
       </c>
       <c r="E28">
-        <v>184</v>
+        <v>51</v>
       </c>
       <c r="F28">
-        <v>736</v>
-      </c>
-      <c r="G28" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" t="s">
-        <v>67</v>
+        <v>131</v>
+      </c>
+      <c r="G28">
+        <v>155</v>
+      </c>
+      <c r="H28">
+        <v>398.1</v>
       </c>
       <c r="I28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J28" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>47</v>
       </c>
       <c r="B29">
-        <v>1987</v>
+        <v>55.206918999999999</v>
       </c>
       <c r="C29">
-        <v>35</v>
+        <v>-132.82456199999999</v>
       </c>
       <c r="D29">
-        <v>110</v>
+        <v>2012</v>
       </c>
       <c r="E29">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="F29">
-        <v>379.1</v>
-      </c>
-      <c r="G29" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" t="s">
-        <v>67</v>
+        <v>119</v>
+      </c>
+      <c r="G29">
+        <v>134</v>
+      </c>
+      <c r="H29">
+        <v>332.2</v>
       </c>
       <c r="I29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J29" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B30">
-        <v>1997</v>
+        <v>55.927008999999998</v>
       </c>
       <c r="C30">
-        <v>51</v>
+        <v>-130.03435899999999</v>
       </c>
       <c r="D30">
-        <v>131</v>
+        <v>1987</v>
       </c>
       <c r="E30">
-        <v>155</v>
+        <v>33</v>
       </c>
       <c r="F30">
-        <v>398.1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" t="s">
-        <v>66</v>
+        <v>39</v>
+      </c>
+      <c r="G30">
+        <v>66</v>
+      </c>
+      <c r="H30">
+        <v>77.900000000000006</v>
       </c>
       <c r="I30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>2012</v>
+        <v>56.97043</v>
       </c>
       <c r="C31">
-        <v>48</v>
+        <v>-133.92920899999999</v>
       </c>
       <c r="D31">
-        <v>119</v>
+        <v>1985</v>
       </c>
       <c r="E31">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="F31">
-        <v>332.2</v>
-      </c>
-      <c r="G31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" t="s">
-        <v>67</v>
+        <v>171</v>
+      </c>
+      <c r="G31">
+        <v>256</v>
+      </c>
+      <c r="H31">
+        <v>625.4</v>
       </c>
       <c r="I31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32">
-        <v>1985</v>
+        <v>56.97043</v>
       </c>
       <c r="C32">
-        <v>70</v>
+        <v>-133.92920899999999</v>
       </c>
       <c r="D32">
-        <v>171</v>
+        <v>1987</v>
       </c>
       <c r="E32">
-        <v>256</v>
+        <v>52</v>
       </c>
       <c r="F32">
-        <v>625.4</v>
-      </c>
-      <c r="G32" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" t="s">
-        <v>67</v>
+        <v>193</v>
+      </c>
+      <c r="G32">
+        <v>192</v>
+      </c>
+      <c r="H32">
+        <v>642</v>
       </c>
       <c r="I32" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
       <c r="B33">
-        <v>1987</v>
+        <v>56.97043</v>
       </c>
       <c r="C33">
-        <v>52</v>
+        <v>-133.92920899999999</v>
       </c>
       <c r="D33">
-        <v>193</v>
+        <v>1996</v>
       </c>
       <c r="E33">
-        <v>192</v>
+        <v>73</v>
       </c>
       <c r="F33">
-        <v>642</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" t="s">
-        <v>67</v>
+        <v>249</v>
+      </c>
+      <c r="G33">
+        <v>219</v>
+      </c>
+      <c r="H33">
+        <v>747</v>
       </c>
       <c r="I33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B34">
-        <v>1996</v>
+        <v>55.541808000000003</v>
       </c>
       <c r="C34">
-        <v>73</v>
+        <v>-132.40832599999999</v>
       </c>
       <c r="D34">
-        <v>249</v>
+        <v>1987</v>
       </c>
       <c r="E34">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="F34">
-        <v>747</v>
-      </c>
-      <c r="G34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" t="s">
-        <v>66</v>
+        <v>14</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="H34">
+        <v>40</v>
       </c>
       <c r="I34" t="s">
+        <v>67</v>
+      </c>
+      <c r="J34" t="s">
+        <v>67</v>
+      </c>
+      <c r="K34" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>43</v>
       </c>
       <c r="B35">
-        <v>1987</v>
+        <v>55.541808000000003</v>
       </c>
       <c r="C35">
+        <v>-132.40832599999999</v>
+      </c>
+      <c r="D35">
+        <v>1998</v>
+      </c>
+      <c r="E35">
         <v>14</v>
       </c>
-      <c r="D35">
-        <v>14</v>
-      </c>
-      <c r="E35">
-        <v>40</v>
-      </c>
       <c r="F35">
-        <v>40</v>
-      </c>
-      <c r="G35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H35" t="s">
-        <v>67</v>
+        <v>18</v>
+      </c>
+      <c r="G35">
+        <v>34</v>
+      </c>
+      <c r="H35">
+        <v>43.7</v>
       </c>
       <c r="I35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" t="s">
+        <v>67</v>
+      </c>
+      <c r="K35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B36">
-        <v>1998</v>
+        <v>55.554183999999999</v>
       </c>
       <c r="C36">
-        <v>14</v>
+        <v>-133.08124799999999</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>1984</v>
       </c>
       <c r="E36">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F36">
-        <v>43.7</v>
-      </c>
-      <c r="G36" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" t="s">
-        <v>67</v>
+        <v>131</v>
+      </c>
+      <c r="G36">
+        <v>130</v>
+      </c>
+      <c r="H36">
+        <v>473.1</v>
       </c>
       <c r="I36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J36" t="s">
+        <v>67</v>
+      </c>
+      <c r="K36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
       <c r="B37">
-        <v>1984</v>
+        <v>55.554183999999999</v>
       </c>
       <c r="C37">
-        <v>36</v>
+        <v>-133.08124799999999</v>
       </c>
       <c r="D37">
-        <v>131</v>
+        <v>1987</v>
       </c>
       <c r="E37">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="F37">
-        <v>473.1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>67</v>
-      </c>
-      <c r="H37" t="s">
-        <v>67</v>
+        <v>224</v>
+      </c>
+      <c r="G37">
+        <v>198</v>
+      </c>
+      <c r="H37">
+        <v>790.3</v>
       </c>
       <c r="I37" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" t="s">
+        <v>67</v>
+      </c>
+      <c r="K37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
       <c r="B38">
-        <v>1987</v>
+        <v>55.554183999999999</v>
       </c>
       <c r="C38">
-        <v>52</v>
+        <v>-133.08124799999999</v>
       </c>
       <c r="D38">
-        <v>224</v>
+        <v>1997</v>
       </c>
       <c r="E38">
-        <v>198</v>
+        <v>106</v>
       </c>
       <c r="F38">
-        <v>790.3</v>
-      </c>
-      <c r="G38" t="s">
-        <v>67</v>
-      </c>
-      <c r="H38" t="s">
-        <v>67</v>
+        <v>303</v>
+      </c>
+      <c r="G38">
+        <v>295</v>
+      </c>
+      <c r="H38">
+        <v>847.3</v>
       </c>
       <c r="I38" t="s">
+        <v>66</v>
+      </c>
+      <c r="J38" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B39">
-        <v>1997</v>
+        <v>59.399774999999998</v>
       </c>
       <c r="C39">
-        <v>106</v>
+        <v>-135.88940199999999</v>
       </c>
       <c r="D39">
-        <v>303</v>
+        <v>1983</v>
       </c>
       <c r="E39">
-        <v>295</v>
+        <v>33</v>
       </c>
       <c r="F39">
-        <v>847.3</v>
-      </c>
-      <c r="G39" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" t="s">
-        <v>66</v>
+        <v>41</v>
+      </c>
+      <c r="G39">
+        <v>124</v>
+      </c>
+      <c r="H39">
+        <v>154.1</v>
       </c>
       <c r="I39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J39" t="s">
+        <v>67</v>
+      </c>
+      <c r="K39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
       <c r="B40">
-        <v>1983</v>
+        <v>59.399774999999998</v>
       </c>
       <c r="C40">
-        <v>33</v>
+        <v>-135.88940199999999</v>
       </c>
       <c r="D40">
-        <v>41</v>
+        <v>1987</v>
       </c>
       <c r="E40">
-        <v>124</v>
+        <v>29</v>
       </c>
       <c r="F40">
-        <v>154.1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>67</v>
-      </c>
-      <c r="H40" t="s">
-        <v>67</v>
+        <v>39</v>
+      </c>
+      <c r="G40">
+        <v>101</v>
+      </c>
+      <c r="H40">
+        <v>133.4</v>
       </c>
       <c r="I40" t="s">
+        <v>67</v>
+      </c>
+      <c r="J40" t="s">
+        <v>67</v>
+      </c>
+      <c r="K40" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
       <c r="B41">
-        <v>1987</v>
+        <v>59.399774999999998</v>
       </c>
       <c r="C41">
-        <v>29</v>
+        <v>-135.88940199999999</v>
       </c>
       <c r="D41">
-        <v>39</v>
+        <v>1996</v>
       </c>
       <c r="E41">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="F41">
-        <v>133.4</v>
-      </c>
-      <c r="G41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H41" t="s">
-        <v>67</v>
+        <v>36</v>
+      </c>
+      <c r="G41">
+        <v>96</v>
+      </c>
+      <c r="H41">
+        <v>108</v>
       </c>
       <c r="I41" t="s">
+        <v>66</v>
+      </c>
+      <c r="J41" t="s">
+        <v>66</v>
+      </c>
+      <c r="K41" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
       <c r="B42">
-        <v>1996</v>
+        <v>59.399774999999998</v>
       </c>
       <c r="C42">
+        <v>-135.88940199999999</v>
+      </c>
+      <c r="D42">
+        <v>2014</v>
+      </c>
+      <c r="E42">
+        <v>24</v>
+      </c>
+      <c r="F42">
         <v>32</v>
       </c>
-      <c r="D42">
-        <v>36</v>
-      </c>
-      <c r="E42">
-        <v>96</v>
-      </c>
-      <c r="F42">
-        <v>108</v>
-      </c>
-      <c r="G42" t="s">
-        <v>66</v>
-      </c>
-      <c r="H42" t="s">
-        <v>66</v>
+      <c r="G42">
+        <v>48</v>
+      </c>
+      <c r="H42">
+        <v>64</v>
       </c>
       <c r="I42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J42" t="s">
+        <v>67</v>
+      </c>
+      <c r="K42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B43">
-        <v>2014</v>
+        <v>55.128414999999997</v>
       </c>
       <c r="C43">
-        <v>24</v>
+        <v>-131.57816399999999</v>
       </c>
       <c r="D43">
-        <v>32</v>
+        <v>1987</v>
       </c>
       <c r="E43">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F43">
-        <v>64</v>
-      </c>
-      <c r="G43" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" t="s">
-        <v>67</v>
+        <v>418</v>
+      </c>
+      <c r="G43">
+        <v>255</v>
+      </c>
+      <c r="H43">
+        <v>1554.2</v>
       </c>
       <c r="I43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J43" t="s">
+        <v>67</v>
+      </c>
+      <c r="K43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>41</v>
       </c>
       <c r="B44">
-        <v>1987</v>
+        <v>55.739387000000001</v>
       </c>
       <c r="C44">
+        <v>-132.25480899999999</v>
+      </c>
+      <c r="D44">
+        <v>1987</v>
+      </c>
+      <c r="E44">
         <v>10</v>
       </c>
-      <c r="D44">
+      <c r="F44">
         <v>10</v>
       </c>
-      <c r="E44">
+      <c r="G44">
         <v>30</v>
       </c>
-      <c r="F44">
+      <c r="H44">
         <v>30</v>
       </c>
-      <c r="G44" t="s">
-        <v>66</v>
-      </c>
-      <c r="H44" t="s">
-        <v>67</v>
-      </c>
       <c r="I44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J44" t="s">
+        <v>67</v>
+      </c>
+      <c r="K44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45">
+        <v>55.869669999999999</v>
+      </c>
+      <c r="C45">
+        <v>-133.19362799999999</v>
+      </c>
+      <c r="D45">
         <v>1998</v>
       </c>
-      <c r="C45">
+      <c r="E45">
         <v>50</v>
       </c>
-      <c r="D45">
-        <v>66</v>
-      </c>
-      <c r="E45">
+      <c r="F45">
+        <v>66</v>
+      </c>
+      <c r="G45">
         <v>111</v>
       </c>
-      <c r="F45">
+      <c r="H45">
         <v>146.5</v>
       </c>
-      <c r="G45" t="s">
-        <v>66</v>
-      </c>
-      <c r="H45" t="s">
-        <v>67</v>
-      </c>
       <c r="I45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J45" t="s">
+        <v>67</v>
+      </c>
+      <c r="K45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>24</v>
       </c>
       <c r="B46">
-        <v>1987</v>
+        <v>57.957799000000001</v>
       </c>
       <c r="C46">
+        <v>-136.21924100000001</v>
+      </c>
+      <c r="D46">
+        <v>1987</v>
+      </c>
+      <c r="E46">
         <v>48</v>
       </c>
-      <c r="D46">
+      <c r="F46">
         <v>82</v>
       </c>
-      <c r="E46">
+      <c r="G46">
         <v>148</v>
       </c>
-      <c r="F46">
+      <c r="H46">
         <v>238.4</v>
       </c>
-      <c r="G46" t="s">
-        <v>66</v>
-      </c>
-      <c r="H46" t="s">
-        <v>67</v>
-      </c>
       <c r="I46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J46" t="s">
+        <v>67</v>
+      </c>
+      <c r="K46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>31</v>
       </c>
       <c r="B47">
-        <v>1987</v>
+        <v>56.803826000000001</v>
       </c>
       <c r="C47">
+        <v>-132.94768300000001</v>
+      </c>
+      <c r="D47">
+        <v>1987</v>
+      </c>
+      <c r="E47">
         <v>49</v>
       </c>
-      <c r="D47">
+      <c r="F47">
         <v>1123</v>
       </c>
-      <c r="E47">
+      <c r="G47">
         <v>166</v>
       </c>
-      <c r="F47">
+      <c r="H47">
         <v>3738.8</v>
       </c>
-      <c r="G47" t="s">
-        <v>67</v>
-      </c>
-      <c r="H47" t="s">
-        <v>67</v>
-      </c>
       <c r="I47" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J47" t="s">
+        <v>67</v>
+      </c>
+      <c r="K47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>
       <c r="B48">
+        <v>56.803826000000001</v>
+      </c>
+      <c r="C48">
+        <v>-132.94768300000001</v>
+      </c>
+      <c r="D48">
         <v>2000</v>
       </c>
-      <c r="C48">
+      <c r="E48">
         <v>125</v>
       </c>
-      <c r="D48">
+      <c r="F48">
         <v>1070</v>
       </c>
-      <c r="E48">
+      <c r="G48">
         <v>344</v>
       </c>
-      <c r="F48">
+      <c r="H48">
         <v>2945</v>
       </c>
-      <c r="G48" t="s">
-        <v>66</v>
-      </c>
-      <c r="H48" t="s">
-        <v>66</v>
-      </c>
       <c r="I48" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J48" t="s">
+        <v>66</v>
+      </c>
+      <c r="K48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>35</v>
       </c>
       <c r="B49">
-        <v>1987</v>
+        <v>56.350473000000001</v>
       </c>
       <c r="C49">
+        <v>-133.62058400000001</v>
+      </c>
+      <c r="D49">
+        <v>1987</v>
+      </c>
+      <c r="E49">
         <v>19</v>
       </c>
-      <c r="D49">
+      <c r="F49">
         <v>19</v>
       </c>
-      <c r="E49">
+      <c r="G49">
         <v>35</v>
       </c>
-      <c r="F49">
+      <c r="H49">
         <v>35</v>
       </c>
-      <c r="G49" t="s">
-        <v>67</v>
-      </c>
-      <c r="H49" t="s">
-        <v>67</v>
-      </c>
       <c r="I49" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J49" t="s">
+        <v>67</v>
+      </c>
+      <c r="K49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>35</v>
       </c>
       <c r="B50">
+        <v>56.350473000000001</v>
+      </c>
+      <c r="C50">
+        <v>-133.62058400000001</v>
+      </c>
+      <c r="D50">
         <v>1996</v>
       </c>
-      <c r="C50">
+      <c r="E50">
         <v>16</v>
       </c>
-      <c r="D50">
+      <c r="F50">
         <v>19</v>
       </c>
-      <c r="E50">
+      <c r="G50">
         <v>40</v>
       </c>
-      <c r="F50">
+      <c r="H50">
         <v>47.5</v>
       </c>
-      <c r="G50" t="s">
-        <v>66</v>
-      </c>
-      <c r="H50" t="s">
-        <v>67</v>
-      </c>
       <c r="I50" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J50" t="s">
+        <v>67</v>
+      </c>
+      <c r="K50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>33</v>
       </c>
       <c r="B51">
-        <v>1987</v>
+        <v>56.25027</v>
       </c>
       <c r="C51">
+        <v>-134.64373000000001</v>
+      </c>
+      <c r="D51">
+        <v>1987</v>
+      </c>
+      <c r="E51">
         <v>34</v>
       </c>
-      <c r="D51">
+      <c r="F51">
         <v>37</v>
       </c>
-      <c r="E51">
+      <c r="G51">
         <v>98</v>
       </c>
-      <c r="F51">
+      <c r="H51">
         <v>106.6</v>
       </c>
-      <c r="G51" t="s">
-        <v>66</v>
-      </c>
-      <c r="H51" t="s">
-        <v>67</v>
-      </c>
       <c r="I51" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J51" t="s">
+        <v>67</v>
+      </c>
+      <c r="K51" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>36</v>
       </c>
       <c r="B52">
-        <v>1987</v>
+        <v>56.319901999999999</v>
       </c>
       <c r="C52">
+        <v>-133.608328</v>
+      </c>
+      <c r="D52">
+        <v>1987</v>
+      </c>
+      <c r="E52">
         <v>25</v>
       </c>
-      <c r="D52">
+      <c r="F52">
         <v>27</v>
       </c>
-      <c r="E52">
+      <c r="G52">
         <v>54</v>
       </c>
-      <c r="F52">
+      <c r="H52">
         <v>58.3</v>
       </c>
-      <c r="G52" t="s">
-        <v>67</v>
-      </c>
-      <c r="H52" t="s">
-        <v>67</v>
-      </c>
       <c r="I52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J52" t="s">
+        <v>67</v>
+      </c>
+      <c r="K52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
       <c r="B53">
+        <v>56.319901999999999</v>
+      </c>
+      <c r="C53">
+        <v>-133.608328</v>
+      </c>
+      <c r="D53">
         <v>1996</v>
-      </c>
-      <c r="C53">
-        <v>25</v>
-      </c>
-      <c r="D53">
-        <v>40</v>
       </c>
       <c r="E53">
         <v>25</v>
       </c>
       <c r="F53">
+        <v>40</v>
+      </c>
+      <c r="G53">
+        <v>25</v>
+      </c>
+      <c r="H53">
         <v>97.5</v>
       </c>
-      <c r="G53" t="s">
-        <v>66</v>
-      </c>
-      <c r="H53" t="s">
-        <v>67</v>
-      </c>
       <c r="I53" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J53" t="s">
+        <v>67</v>
+      </c>
+      <c r="K53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
       <c r="B54">
-        <v>1987</v>
+        <v>55.318365999999997</v>
       </c>
       <c r="C54">
+        <v>-131.593603</v>
+      </c>
+      <c r="D54">
+        <v>1987</v>
+      </c>
+      <c r="E54">
         <v>36</v>
       </c>
-      <c r="D54">
+      <c r="F54">
         <v>76</v>
       </c>
-      <c r="E54">
+      <c r="G54">
         <v>127</v>
       </c>
-      <c r="F54">
+      <c r="H54">
         <v>258.7</v>
       </c>
-      <c r="G54" t="s">
-        <v>67</v>
-      </c>
-      <c r="H54" t="s">
-        <v>67</v>
-      </c>
       <c r="I54" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J54" t="s">
+        <v>67</v>
+      </c>
+      <c r="K54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>49</v>
       </c>
       <c r="B55">
+        <v>55.318365999999997</v>
+      </c>
+      <c r="C55">
+        <v>-131.593603</v>
+      </c>
+      <c r="D55">
         <v>1999</v>
       </c>
-      <c r="C55">
+      <c r="E55">
         <v>73</v>
       </c>
-      <c r="D55">
+      <c r="F55">
         <v>110</v>
       </c>
-      <c r="E55">
+      <c r="G55">
         <v>252</v>
       </c>
-      <c r="F55">
+      <c r="H55">
         <v>379.7</v>
       </c>
-      <c r="G55" t="s">
-        <v>66</v>
-      </c>
-      <c r="H55" t="s">
-        <v>67</v>
-      </c>
       <c r="I55" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J55" t="s">
+        <v>67</v>
+      </c>
+      <c r="K55" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>27</v>
       </c>
       <c r="B56">
-        <v>1987</v>
+        <v>57.053023000000003</v>
       </c>
       <c r="C56">
+        <v>-135.325489</v>
+      </c>
+      <c r="D56">
+        <v>1987</v>
+      </c>
+      <c r="E56">
         <v>296</v>
       </c>
-      <c r="D56">
+      <c r="F56">
         <v>2871</v>
       </c>
-      <c r="E56">
+      <c r="G56">
         <v>831</v>
       </c>
-      <c r="F56">
+      <c r="H56">
         <v>8060.7</v>
       </c>
-      <c r="G56" t="s">
-        <v>67</v>
-      </c>
-      <c r="H56" t="s">
-        <v>67</v>
-      </c>
       <c r="I56" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J56" t="s">
+        <v>67</v>
+      </c>
+      <c r="K56" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>27</v>
       </c>
       <c r="B57">
+        <v>57.053023000000003</v>
+      </c>
+      <c r="C57">
+        <v>-135.325489</v>
+      </c>
+      <c r="D57">
         <v>1996</v>
       </c>
-      <c r="C57">
+      <c r="E57">
         <v>150</v>
       </c>
-      <c r="D57">
+      <c r="F57">
         <v>3053</v>
       </c>
-      <c r="E57">
+      <c r="G57">
         <v>431</v>
       </c>
-      <c r="F57">
+      <c r="H57">
         <v>8535</v>
       </c>
-      <c r="G57" t="s">
-        <v>67</v>
-      </c>
-      <c r="H57" t="s">
-        <v>66</v>
-      </c>
       <c r="I57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J57" t="s">
+        <v>66</v>
+      </c>
+      <c r="K57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>27</v>
       </c>
       <c r="B58">
+        <v>57.053023000000003</v>
+      </c>
+      <c r="C58">
+        <v>-135.325489</v>
+      </c>
+      <c r="D58">
         <v>2013</v>
       </c>
-      <c r="C58">
+      <c r="E58">
         <v>212</v>
       </c>
-      <c r="D58">
+      <c r="F58">
         <v>2965</v>
       </c>
-      <c r="E58">
+      <c r="G58">
         <v>592</v>
       </c>
-      <c r="F58">
+      <c r="H58">
         <v>7873.2</v>
       </c>
-      <c r="G58" t="s">
-        <v>66</v>
-      </c>
-      <c r="H58" t="s">
-        <v>67</v>
-      </c>
       <c r="I58" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J58" t="s">
+        <v>67</v>
+      </c>
+      <c r="K58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
       <c r="B59">
-        <v>1987</v>
+        <v>59.451850999999998</v>
       </c>
       <c r="C59">
+        <v>-135.31772599999999</v>
+      </c>
+      <c r="D59">
+        <v>1987</v>
+      </c>
+      <c r="E59">
         <v>60</v>
       </c>
-      <c r="D59">
+      <c r="F59">
         <v>204</v>
       </c>
-      <c r="E59">
+      <c r="G59">
         <v>164</v>
       </c>
-      <c r="F59">
+      <c r="H59">
         <v>582.6</v>
       </c>
-      <c r="G59" t="s">
-        <v>66</v>
-      </c>
-      <c r="H59" t="s">
-        <v>67</v>
-      </c>
       <c r="I59" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J59" t="s">
+        <v>67</v>
+      </c>
+      <c r="K59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>23</v>
       </c>
       <c r="B60">
+        <v>57.781731999999998</v>
+      </c>
+      <c r="C60">
+        <v>-135.202494</v>
+      </c>
+      <c r="D60">
         <v>1984</v>
       </c>
-      <c r="C60">
+      <c r="E60">
         <v>24</v>
       </c>
-      <c r="D60">
+      <c r="F60">
         <v>47</v>
       </c>
-      <c r="E60">
+      <c r="G60">
         <v>48</v>
       </c>
-      <c r="F60">
+      <c r="H60">
         <v>94</v>
       </c>
-      <c r="G60" t="s">
-        <v>67</v>
-      </c>
-      <c r="H60" t="s">
-        <v>67</v>
-      </c>
       <c r="I60" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J60" t="s">
+        <v>67</v>
+      </c>
+      <c r="K60" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>23</v>
       </c>
       <c r="B61">
-        <v>1987</v>
+        <v>57.781731999999998</v>
       </c>
       <c r="C61">
+        <v>-135.202494</v>
+      </c>
+      <c r="D61">
+        <v>1987</v>
+      </c>
+      <c r="E61">
         <v>31</v>
       </c>
-      <c r="D61">
+      <c r="F61">
         <v>44</v>
       </c>
-      <c r="E61">
-        <v>66</v>
-      </c>
-      <c r="F61">
+      <c r="G61">
+        <v>66</v>
+      </c>
+      <c r="H61">
         <v>94.7</v>
       </c>
-      <c r="G61" t="s">
-        <v>66</v>
-      </c>
-      <c r="H61" t="s">
-        <v>67</v>
-      </c>
       <c r="I61" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J61" t="s">
+        <v>67</v>
+      </c>
+      <c r="K61" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
       <c r="B62">
-        <v>1987</v>
+        <v>55.681398999999999</v>
       </c>
       <c r="C62">
+        <v>-132.51284899999999</v>
+      </c>
+      <c r="D62">
+        <v>1987</v>
+      </c>
+      <c r="E62">
         <v>52</v>
       </c>
-      <c r="D62">
+      <c r="F62">
         <v>157</v>
       </c>
-      <c r="E62">
+      <c r="G62">
         <v>163</v>
       </c>
-      <c r="F62">
+      <c r="H62">
         <v>478.5</v>
       </c>
-      <c r="G62" t="s">
-        <v>67</v>
-      </c>
-      <c r="H62" t="s">
-        <v>67</v>
-      </c>
       <c r="I62" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J62" t="s">
+        <v>67</v>
+      </c>
+      <c r="K62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>42</v>
       </c>
       <c r="B63">
+        <v>55.681398999999999</v>
+      </c>
+      <c r="C63">
+        <v>-132.51284899999999</v>
+      </c>
+      <c r="D63">
         <v>1998</v>
       </c>
-      <c r="C63">
+      <c r="E63">
         <v>89</v>
       </c>
-      <c r="D63">
+      <c r="F63">
         <v>204</v>
       </c>
-      <c r="E63">
+      <c r="G63">
         <v>226</v>
       </c>
-      <c r="F63">
+      <c r="H63">
         <v>518</v>
       </c>
-      <c r="G63" t="s">
-        <v>66</v>
-      </c>
-      <c r="H63" t="s">
-        <v>67</v>
-      </c>
       <c r="I63" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J63" t="s">
+        <v>67</v>
+      </c>
+      <c r="K63" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>38</v>
       </c>
       <c r="B64">
-        <v>1987</v>
+        <v>56.122591</v>
       </c>
       <c r="C64">
+        <v>-133.12890100000001</v>
+      </c>
+      <c r="D64">
+        <v>1987</v>
+      </c>
+      <c r="E64">
         <v>18</v>
       </c>
-      <c r="D64">
+      <c r="F64">
         <v>18</v>
       </c>
-      <c r="E64">
+      <c r="G64">
         <v>51</v>
       </c>
-      <c r="F64">
+      <c r="H64">
         <v>51</v>
       </c>
-      <c r="G64" t="s">
-        <v>67</v>
-      </c>
-      <c r="H64" t="s">
-        <v>67</v>
-      </c>
       <c r="I64" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J64" t="s">
+        <v>67</v>
+      </c>
+      <c r="K64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
       <c r="B65">
+        <v>56.122591</v>
+      </c>
+      <c r="C65">
+        <v>-133.12890100000001</v>
+      </c>
+      <c r="D65">
         <v>1998</v>
       </c>
-      <c r="C65">
+      <c r="E65">
         <v>15</v>
       </c>
-      <c r="D65">
+      <c r="F65">
         <v>20</v>
       </c>
-      <c r="E65">
+      <c r="G65">
         <v>41</v>
       </c>
-      <c r="F65">
+      <c r="H65">
         <v>54.7</v>
       </c>
-      <c r="G65" t="s">
-        <v>67</v>
-      </c>
-      <c r="H65" t="s">
-        <v>67</v>
-      </c>
       <c r="I65" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J65" t="s">
+        <v>67</v>
+      </c>
+      <c r="K65" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
       <c r="B66">
+        <v>56.122591</v>
+      </c>
+      <c r="C66">
+        <v>-133.12890100000001</v>
+      </c>
+      <c r="D66">
         <v>2012</v>
       </c>
-      <c r="C66">
+      <c r="E66">
         <v>21</v>
       </c>
-      <c r="D66">
+      <c r="F66">
         <v>27</v>
       </c>
-      <c r="E66">
+      <c r="G66">
         <v>43</v>
       </c>
-      <c r="F66">
+      <c r="H66">
         <v>55.3</v>
       </c>
-      <c r="G66" t="s">
-        <v>66</v>
-      </c>
-      <c r="H66" t="s">
-        <v>67</v>
-      </c>
       <c r="I66" t="s">
+        <v>66</v>
+      </c>
+      <c r="J66" t="s">
+        <v>67</v>
+      </c>
+      <c r="K66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B67">
+        <v>58.087257999999999</v>
+      </c>
+      <c r="C67">
+        <v>-135.43440100000001</v>
+      </c>
+      <c r="D67">
+        <v>1996</v>
+      </c>
+      <c r="E67">
+        <v>24</v>
+      </c>
+      <c r="F67">
+        <v>41</v>
+      </c>
+      <c r="G67">
+        <v>83</v>
+      </c>
+      <c r="H67">
+        <v>141.80000000000001</v>
+      </c>
+      <c r="I67" t="s">
+        <v>66</v>
+      </c>
+      <c r="J67" t="s">
+        <v>67</v>
+      </c>
+      <c r="K67" t="s">
         <v>162</v>
       </c>
-      <c r="B67">
-        <v>1996</v>
-      </c>
-      <c r="C67">
-        <v>24</v>
-      </c>
-      <c r="D67">
-        <v>41</v>
-      </c>
-      <c r="E67">
-        <v>83</v>
-      </c>
-      <c r="F67">
-        <v>141.80000000000001</v>
-      </c>
-      <c r="G67" t="s">
-        <v>66</v>
-      </c>
-      <c r="H67" t="s">
-        <v>67</v>
-      </c>
-      <c r="I67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>34</v>
       </c>
       <c r="B68">
-        <v>1987</v>
+        <v>56.466940999999998</v>
       </c>
       <c r="C68">
+        <v>-132.36551600000001</v>
+      </c>
+      <c r="D68">
+        <v>1987</v>
+      </c>
+      <c r="E68">
         <v>75</v>
       </c>
-      <c r="D68">
+      <c r="F68">
         <v>1013</v>
       </c>
-      <c r="E68">
+      <c r="G68">
         <v>211</v>
       </c>
-      <c r="F68">
+      <c r="H68">
         <v>2839</v>
       </c>
-      <c r="G68" t="s">
-        <v>67</v>
-      </c>
-      <c r="H68" t="s">
-        <v>67</v>
-      </c>
       <c r="I68" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J68" t="s">
+        <v>67</v>
+      </c>
+      <c r="K68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>34</v>
       </c>
       <c r="B69">
+        <v>56.466940999999998</v>
+      </c>
+      <c r="C69">
+        <v>-132.36551600000001</v>
+      </c>
+      <c r="D69">
         <v>2000</v>
       </c>
-      <c r="C69">
+      <c r="E69">
         <v>98</v>
       </c>
-      <c r="D69">
+      <c r="F69">
         <v>747</v>
       </c>
-      <c r="E69">
+      <c r="G69">
         <v>257</v>
       </c>
-      <c r="F69">
+      <c r="H69">
         <v>1959</v>
       </c>
-      <c r="G69" t="s">
-        <v>66</v>
-      </c>
-      <c r="H69" t="s">
-        <v>66</v>
-      </c>
       <c r="I69" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J69" t="s">
+        <v>66</v>
+      </c>
+      <c r="K69" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>3</v>
       </c>
       <c r="B70">
+        <v>59.554414999999999</v>
+      </c>
+      <c r="C70">
+        <v>-139.718794</v>
+      </c>
+      <c r="D70">
         <v>1984</v>
       </c>
-      <c r="C70">
+      <c r="E70">
         <v>50</v>
       </c>
-      <c r="D70">
+      <c r="F70">
         <v>181</v>
       </c>
-      <c r="E70">
+      <c r="G70">
         <v>150</v>
       </c>
-      <c r="F70">
+      <c r="H70">
         <v>543</v>
       </c>
-      <c r="G70" t="s">
-        <v>67</v>
-      </c>
-      <c r="H70" t="s">
-        <v>67</v>
-      </c>
       <c r="I70" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J70" t="s">
+        <v>67</v>
+      </c>
+      <c r="K70" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>3</v>
       </c>
       <c r="B71">
-        <v>1987</v>
+        <v>59.554414999999999</v>
       </c>
       <c r="C71">
+        <v>-139.718794</v>
+      </c>
+      <c r="D71">
+        <v>1987</v>
+      </c>
+      <c r="E71">
         <v>48</v>
       </c>
-      <c r="D71">
+      <c r="F71">
         <v>169</v>
       </c>
-      <c r="E71">
+      <c r="G71">
         <v>184</v>
       </c>
-      <c r="F71">
+      <c r="H71">
         <v>588.79999999999995</v>
       </c>
-      <c r="G71" t="s">
-        <v>67</v>
-      </c>
-      <c r="H71" t="s">
-        <v>67</v>
-      </c>
       <c r="I71" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="J71" t="s">
+        <v>67</v>
+      </c>
+      <c r="K71" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>3</v>
       </c>
       <c r="B72">
+        <v>59.554414999999999</v>
+      </c>
+      <c r="C72">
+        <v>-139.718794</v>
+      </c>
+      <c r="D72">
         <v>2000</v>
       </c>
-      <c r="C72">
+      <c r="E72">
         <v>139</v>
       </c>
-      <c r="D72">
+      <c r="F72">
         <v>234</v>
       </c>
-      <c r="E72">
+      <c r="G72">
         <v>377</v>
       </c>
-      <c r="F72">
+      <c r="H72">
         <v>634.70000000000005</v>
       </c>
-      <c r="G72" t="s">
-        <v>66</v>
-      </c>
-      <c r="H72" t="s">
-        <v>66</v>
-      </c>
       <c r="I72" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="J72" t="s">
+        <v>66</v>
+      </c>
+      <c r="K72" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>3</v>
       </c>
       <c r="B73">
+        <v>59.554414999999999</v>
+      </c>
+      <c r="C73">
+        <v>-139.718794</v>
+      </c>
+      <c r="D73">
         <v>2015</v>
       </c>
-      <c r="C73">
+      <c r="E73">
         <v>101</v>
       </c>
-      <c r="D73">
+      <c r="F73">
         <v>240</v>
       </c>
-      <c r="E73">
+      <c r="G73">
         <v>249</v>
       </c>
-      <c r="F73">
+      <c r="H73">
         <v>591.70000000000005</v>
       </c>
-      <c r="G73" t="s">
-        <v>66</v>
-      </c>
-      <c r="H73" t="s">
-        <v>67</v>
-      </c>
       <c r="I73" t="s">
-        <v>101</v>
+        <v>66</v>
+      </c>
+      <c r="J73" t="s">
+        <v>67</v>
+      </c>
+      <c r="K73" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I73" xr:uid="{DB7C6250-0454-1242-8FEF-5BAB633824E4}"/>
+  <autoFilter ref="A1:K73" xr:uid="{DB7C6250-0454-1242-8FEF-5BAB633824E4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K73">
+      <sortCondition ref="A1:A73"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>